<commit_message>
Number of factors addressed by study
</commit_message>
<xml_diff>
--- a/data/References_used_for_review.xlsx
+++ b/data/References_used_for_review.xlsx
@@ -8,16 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aponchon\Nextcloud\Aurore\Projects\Prospecting review\Prospecting-review-analysis\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25E06AC5-CA48-4DD2-BAD0-9DE0F2D7722C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB8DD3CA-F759-4C8A-9891-FF52EA75C969}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Supp_1" sheetId="4" r:id="rId1"/>
     <sheet name="Factors_adressed" sheetId="5" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Factors_adressed!$A$1:$X$125</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Factors_adressed!$A$1:$Y$125</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Supp_1!$A$1:$X$125</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2813" uniqueCount="748">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2813" uniqueCount="750">
   <si>
     <t>Species</t>
   </si>
@@ -2538,6 +2538,12 @@
       </rPr>
       <t xml:space="preserve"> Inbreeding + dispersal status</t>
     </r>
+  </si>
+  <si>
+    <t>Ponchon -a</t>
+  </si>
+  <si>
+    <t>Ponchon -b</t>
   </si>
 </sst>
 </file>
@@ -2849,7 +2855,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="105">
+  <cellXfs count="107">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
@@ -2959,6 +2965,8 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Lien hypertexte" xfId="1" builtinId="8"/>
@@ -3256,7 +3264,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BD4A6C70-8507-4B4A-8FF8-89379E8F198D}">
   <dimension ref="A1:DS125"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <pane xSplit="12" ySplit="27" topLeftCell="M28" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="L1" sqref="L1"/>
       <selection pane="bottomLeft" activeCell="A28" sqref="A28"/>
@@ -12246,11 +12254,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4A5772B6-064D-45BE-A42A-53D0AD546609}">
-  <dimension ref="A1:X127"/>
+  <dimension ref="A1:Y127"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="O4" sqref="O4:O97"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A59" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B84" sqref="B84"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12272,14 +12280,14 @@
     <col min="15" max="15" width="10.42578125" style="50" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="12" style="50" customWidth="1"/>
     <col min="17" max="17" width="4.85546875" style="50" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="6.85546875" style="50" customWidth="1"/>
-    <col min="20" max="20" width="10.7109375" style="50" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="14.85546875" style="50" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="38.85546875" style="50" bestFit="1" customWidth="1"/>
-    <col min="23" max="24" width="11.42578125" style="50"/>
+    <col min="18" max="19" width="6.85546875" style="50" customWidth="1"/>
+    <col min="21" max="21" width="10.7109375" style="50" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="14.85546875" style="50" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="38.85546875" style="50" bestFit="1" customWidth="1"/>
+    <col min="24" max="25" width="11.42578125" style="50"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>6</v>
       </c>
@@ -12334,17 +12342,18 @@
       <c r="R1" s="61" t="s">
         <v>677</v>
       </c>
-      <c r="T1" s="36" t="s">
+      <c r="S1" s="105"/>
+      <c r="U1" s="36" t="s">
         <v>618</v>
       </c>
-      <c r="U1" s="8" t="s">
+      <c r="V1" s="8" t="s">
         <v>611</v>
       </c>
-      <c r="V1"/>
       <c r="W1"/>
       <c r="X1"/>
-    </row>
-    <row r="2" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="Y1"/>
+    </row>
+    <row r="2" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A2" s="13">
         <v>1</v>
       </c>
@@ -12397,22 +12406,26 @@
         <v>0</v>
       </c>
       <c r="R2" s="62">
-        <f>SUM(T2:U2)</f>
-        <v>0</v>
-      </c>
-      <c r="T2" s="37">
-        <v>0</v>
-      </c>
-      <c r="U2" s="16">
-        <v>0</v>
-      </c>
-      <c r="V2" s="51" t="s">
+        <f>SUM(U2:V2)</f>
+        <v>0</v>
+      </c>
+      <c r="T2" s="106">
+        <f>SUM(H2:R2)</f>
+        <v>3</v>
+      </c>
+      <c r="U2" s="37">
+        <v>0</v>
+      </c>
+      <c r="V2" s="16">
+        <v>0</v>
+      </c>
+      <c r="W2" s="51" t="s">
         <v>668</v>
       </c>
-      <c r="W2"/>
       <c r="X2"/>
-    </row>
-    <row r="3" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="Y2"/>
+    </row>
+    <row r="3" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A3" s="13">
         <v>2</v>
       </c>
@@ -12465,22 +12478,26 @@
         <v>0</v>
       </c>
       <c r="R3" s="62">
-        <f t="shared" ref="R3:R66" si="0">SUM(T3:U3)</f>
-        <v>0</v>
-      </c>
-      <c r="T3" s="37">
-        <v>0</v>
-      </c>
-      <c r="U3" s="16">
-        <v>0</v>
-      </c>
-      <c r="V3" s="52" t="s">
+        <f t="shared" ref="R3:R66" si="0">SUM(U3:V3)</f>
+        <v>0</v>
+      </c>
+      <c r="T3" s="106">
+        <f t="shared" ref="T3:T66" si="1">SUM(H3:R3)</f>
+        <v>2</v>
+      </c>
+      <c r="U3" s="37">
+        <v>0</v>
+      </c>
+      <c r="V3" s="16">
+        <v>0</v>
+      </c>
+      <c r="W3" s="52" t="s">
         <v>669</v>
       </c>
-      <c r="W3"/>
       <c r="X3"/>
-    </row>
-    <row r="4" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="Y3"/>
+    </row>
+    <row r="4" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A4" s="13">
         <v>3</v>
       </c>
@@ -12536,19 +12553,23 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="T4" s="37">
-        <v>0</v>
-      </c>
-      <c r="U4" s="16">
-        <v>0</v>
-      </c>
-      <c r="V4" s="4" t="s">
+      <c r="T4" s="106">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="U4" s="37">
+        <v>0</v>
+      </c>
+      <c r="V4" s="16">
+        <v>0</v>
+      </c>
+      <c r="W4" s="4" t="s">
         <v>670</v>
       </c>
-      <c r="W4"/>
       <c r="X4"/>
-    </row>
-    <row r="5" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="Y4"/>
+    </row>
+    <row r="5" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A5" s="13">
         <v>4</v>
       </c>
@@ -12604,19 +12625,23 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="T5" s="37">
-        <v>0</v>
-      </c>
-      <c r="U5" s="16">
-        <v>0</v>
-      </c>
-      <c r="V5" s="53" t="s">
+      <c r="T5" s="106">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="U5" s="37">
+        <v>0</v>
+      </c>
+      <c r="V5" s="16">
+        <v>0</v>
+      </c>
+      <c r="W5" s="53" t="s">
         <v>671</v>
       </c>
-      <c r="W5"/>
       <c r="X5"/>
-    </row>
-    <row r="6" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="Y5"/>
+    </row>
+    <row r="6" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A6" s="13">
         <v>5</v>
       </c>
@@ -12672,19 +12697,23 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="T6" s="37">
-        <v>0</v>
-      </c>
-      <c r="U6" s="16">
-        <v>0</v>
-      </c>
-      <c r="V6" s="54" t="s">
+      <c r="T6" s="106">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="U6" s="37">
+        <v>0</v>
+      </c>
+      <c r="V6" s="16">
+        <v>0</v>
+      </c>
+      <c r="W6" s="54" t="s">
         <v>673</v>
       </c>
-      <c r="W6"/>
       <c r="X6"/>
-    </row>
-    <row r="7" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="Y6"/>
+    </row>
+    <row r="7" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A7" s="13">
         <v>6</v>
       </c>
@@ -12740,19 +12769,23 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="T7" s="37">
-        <v>0</v>
-      </c>
-      <c r="U7" s="16">
-        <v>0</v>
-      </c>
-      <c r="V7" s="55" t="s">
+      <c r="T7" s="106">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
+      <c r="U7" s="37">
+        <v>0</v>
+      </c>
+      <c r="V7" s="16">
+        <v>0</v>
+      </c>
+      <c r="W7" s="55" t="s">
         <v>674</v>
       </c>
-      <c r="W7"/>
       <c r="X7"/>
-    </row>
-    <row r="8" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="Y7"/>
+    </row>
+    <row r="8" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A8" s="13">
         <v>7</v>
       </c>
@@ -12808,19 +12841,23 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="T8" s="37">
-        <v>0</v>
-      </c>
-      <c r="U8" s="16">
-        <v>0</v>
-      </c>
-      <c r="V8" s="56" t="s">
+      <c r="T8" s="106">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="U8" s="37">
+        <v>0</v>
+      </c>
+      <c r="V8" s="16">
+        <v>0</v>
+      </c>
+      <c r="W8" s="56" t="s">
         <v>672</v>
       </c>
-      <c r="W8"/>
       <c r="X8"/>
-    </row>
-    <row r="9" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="Y8"/>
+    </row>
+    <row r="9" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A9" s="13">
         <v>8</v>
       </c>
@@ -12876,19 +12913,23 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="T9" s="37">
-        <v>0</v>
-      </c>
-      <c r="U9" s="16">
-        <v>0</v>
-      </c>
-      <c r="V9" s="57" t="s">
+      <c r="T9" s="106">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
+      <c r="U9" s="37">
+        <v>0</v>
+      </c>
+      <c r="V9" s="16">
+        <v>0</v>
+      </c>
+      <c r="W9" s="57" t="s">
         <v>675</v>
       </c>
-      <c r="W9"/>
       <c r="X9"/>
-    </row>
-    <row r="10" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="Y9"/>
+    </row>
+    <row r="10" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A10" s="13">
         <v>9</v>
       </c>
@@ -12944,19 +12985,23 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="T10" s="37">
-        <v>0</v>
-      </c>
-      <c r="U10" s="16">
-        <v>0</v>
-      </c>
-      <c r="V10" s="34" t="s">
+      <c r="T10" s="106">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="U10" s="37">
+        <v>0</v>
+      </c>
+      <c r="V10" s="16">
+        <v>0</v>
+      </c>
+      <c r="W10" s="34" t="s">
         <v>676</v>
       </c>
-      <c r="W10"/>
       <c r="X10"/>
-    </row>
-    <row r="11" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="Y10"/>
+    </row>
+    <row r="11" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A11" s="13">
         <v>10</v>
       </c>
@@ -13012,19 +13057,23 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="T11" s="37">
-        <v>0</v>
-      </c>
-      <c r="U11" s="16">
-        <v>0</v>
-      </c>
-      <c r="V11" s="58" t="s">
+      <c r="T11" s="106">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="U11" s="37">
+        <v>0</v>
+      </c>
+      <c r="V11" s="16">
+        <v>0</v>
+      </c>
+      <c r="W11" s="58" t="s">
         <v>678</v>
       </c>
-      <c r="W11"/>
       <c r="X11"/>
-    </row>
-    <row r="12" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="Y11"/>
+    </row>
+    <row r="12" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A12" s="13">
         <v>11</v>
       </c>
@@ -13080,19 +13129,23 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="T12" s="37">
-        <v>0</v>
-      </c>
-      <c r="U12" s="16">
-        <v>0</v>
-      </c>
-      <c r="V12" s="59" t="s">
+      <c r="T12" s="106">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="U12" s="37">
+        <v>0</v>
+      </c>
+      <c r="V12" s="16">
+        <v>0</v>
+      </c>
+      <c r="W12" s="59" t="s">
         <v>745</v>
       </c>
-      <c r="W12"/>
       <c r="X12"/>
-    </row>
-    <row r="13" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="Y12"/>
+    </row>
+    <row r="13" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A13" s="13">
         <v>12</v>
       </c>
@@ -13148,19 +13201,23 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="T13" s="37">
-        <v>0</v>
-      </c>
-      <c r="U13" s="16">
-        <v>0</v>
-      </c>
-      <c r="V13" s="67" t="s">
+      <c r="T13" s="106">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="U13" s="37">
+        <v>0</v>
+      </c>
+      <c r="V13" s="16">
+        <v>0</v>
+      </c>
+      <c r="W13" s="67" t="s">
         <v>746</v>
       </c>
-      <c r="W13"/>
       <c r="X13"/>
-    </row>
-    <row r="14" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="Y13"/>
+    </row>
+    <row r="14" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A14" s="13">
         <v>13</v>
       </c>
@@ -13216,16 +13273,20 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="T14" s="37">
-        <v>0</v>
-      </c>
-      <c r="U14" s="16">
-        <v>0</v>
-      </c>
-      <c r="W14"/>
+      <c r="T14" s="106">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="U14" s="37">
+        <v>0</v>
+      </c>
+      <c r="V14" s="16">
+        <v>0</v>
+      </c>
       <c r="X14"/>
-    </row>
-    <row r="15" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="Y14"/>
+    </row>
+    <row r="15" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A15" s="13">
         <v>14</v>
       </c>
@@ -13281,19 +13342,23 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="T15" s="37">
-        <v>0</v>
-      </c>
-      <c r="U15" s="16">
-        <v>0</v>
-      </c>
-      <c r="V15" s="60" t="s">
+      <c r="T15" s="106">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
+      <c r="U15" s="37">
+        <v>0</v>
+      </c>
+      <c r="V15" s="16">
+        <v>0</v>
+      </c>
+      <c r="W15" s="60" t="s">
         <v>747</v>
       </c>
-      <c r="W15"/>
       <c r="X15"/>
-    </row>
-    <row r="16" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="Y15"/>
+    </row>
+    <row r="16" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A16" s="13">
         <v>15</v>
       </c>
@@ -13349,16 +13414,20 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="T16" s="37">
-        <v>0</v>
-      </c>
-      <c r="U16" s="16">
-        <v>0</v>
-      </c>
-      <c r="W16"/>
+      <c r="T16" s="106">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="U16" s="37">
+        <v>0</v>
+      </c>
+      <c r="V16" s="16">
+        <v>0</v>
+      </c>
       <c r="X16"/>
-    </row>
-    <row r="17" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="Y16"/>
+    </row>
+    <row r="17" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A17" s="23">
         <v>16</v>
       </c>
@@ -13414,17 +13483,21 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="T17" s="37">
-        <v>0</v>
-      </c>
-      <c r="U17" s="16">
-        <v>0</v>
-      </c>
-      <c r="V17"/>
+      <c r="T17" s="106">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="U17" s="37">
+        <v>0</v>
+      </c>
+      <c r="V17" s="16">
+        <v>0</v>
+      </c>
       <c r="W17"/>
       <c r="X17"/>
-    </row>
-    <row r="18" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="Y17"/>
+    </row>
+    <row r="18" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A18" s="13">
         <v>17</v>
       </c>
@@ -13480,17 +13553,21 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="T18" s="37">
-        <v>0</v>
-      </c>
-      <c r="U18" s="16">
-        <v>0</v>
-      </c>
-      <c r="V18"/>
+      <c r="T18" s="106">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="U18" s="37">
+        <v>0</v>
+      </c>
+      <c r="V18" s="16">
+        <v>0</v>
+      </c>
       <c r="W18"/>
       <c r="X18"/>
-    </row>
-    <row r="19" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="Y18"/>
+    </row>
+    <row r="19" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A19" s="23">
         <v>18</v>
       </c>
@@ -13546,17 +13623,21 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="T19" s="37">
-        <v>0</v>
-      </c>
-      <c r="U19" s="16">
-        <v>0</v>
-      </c>
-      <c r="V19"/>
+      <c r="T19" s="106">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
+      <c r="U19" s="37">
+        <v>0</v>
+      </c>
+      <c r="V19" s="16">
+        <v>0</v>
+      </c>
       <c r="W19"/>
       <c r="X19"/>
-    </row>
-    <row r="20" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="Y19"/>
+    </row>
+    <row r="20" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A20" s="23">
         <v>19</v>
       </c>
@@ -13612,17 +13693,21 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="T20" s="37">
-        <v>0</v>
-      </c>
-      <c r="U20" s="16">
-        <v>0</v>
-      </c>
-      <c r="V20"/>
+      <c r="T20" s="106">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="U20" s="37">
+        <v>0</v>
+      </c>
+      <c r="V20" s="16">
+        <v>0</v>
+      </c>
       <c r="W20"/>
       <c r="X20"/>
-    </row>
-    <row r="21" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="Y20"/>
+    </row>
+    <row r="21" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A21" s="13">
         <v>20</v>
       </c>
@@ -13678,17 +13763,21 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="T21" s="37">
-        <v>0</v>
-      </c>
-      <c r="U21" s="16">
-        <v>0</v>
-      </c>
-      <c r="V21"/>
+      <c r="T21" s="106">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="U21" s="37">
+        <v>0</v>
+      </c>
+      <c r="V21" s="16">
+        <v>0</v>
+      </c>
       <c r="W21"/>
       <c r="X21"/>
-    </row>
-    <row r="22" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="Y21"/>
+    </row>
+    <row r="22" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A22" s="13">
         <v>21</v>
       </c>
@@ -13744,17 +13833,21 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="T22" s="37">
-        <v>0</v>
-      </c>
-      <c r="U22" s="16">
-        <v>0</v>
-      </c>
-      <c r="V22"/>
+      <c r="T22" s="106">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
+      <c r="U22" s="37">
+        <v>0</v>
+      </c>
+      <c r="V22" s="16">
+        <v>0</v>
+      </c>
       <c r="W22"/>
       <c r="X22"/>
-    </row>
-    <row r="23" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="Y22"/>
+    </row>
+    <row r="23" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A23" s="13">
         <v>22</v>
       </c>
@@ -13810,17 +13903,21 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="T23" s="37">
-        <v>0</v>
-      </c>
-      <c r="U23" s="16">
-        <v>0</v>
-      </c>
-      <c r="V23"/>
+      <c r="T23" s="106">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="U23" s="37">
+        <v>0</v>
+      </c>
+      <c r="V23" s="16">
+        <v>0</v>
+      </c>
       <c r="W23"/>
       <c r="X23"/>
-    </row>
-    <row r="24" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="Y23"/>
+    </row>
+    <row r="24" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A24" s="13">
         <v>23</v>
       </c>
@@ -13876,17 +13973,21 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="T24" s="37">
-        <v>0</v>
-      </c>
-      <c r="U24" s="16">
-        <v>0</v>
-      </c>
-      <c r="V24"/>
+      <c r="T24" s="106">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="U24" s="37">
+        <v>0</v>
+      </c>
+      <c r="V24" s="16">
+        <v>0</v>
+      </c>
       <c r="W24"/>
       <c r="X24"/>
-    </row>
-    <row r="25" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="Y24"/>
+    </row>
+    <row r="25" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A25" s="13">
         <v>24</v>
       </c>
@@ -13942,17 +14043,21 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="T25" s="37">
-        <v>0</v>
-      </c>
-      <c r="U25" s="16">
-        <v>0</v>
-      </c>
-      <c r="V25"/>
+      <c r="T25" s="106">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="U25" s="37">
+        <v>0</v>
+      </c>
+      <c r="V25" s="16">
+        <v>0</v>
+      </c>
       <c r="W25"/>
       <c r="X25"/>
-    </row>
-    <row r="26" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="Y25"/>
+    </row>
+    <row r="26" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A26" s="13">
         <v>25</v>
       </c>
@@ -14008,17 +14113,21 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="T26" s="37">
-        <v>0</v>
-      </c>
-      <c r="U26" s="16">
-        <v>0</v>
-      </c>
-      <c r="V26"/>
+      <c r="T26" s="106">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="U26" s="37">
+        <v>0</v>
+      </c>
+      <c r="V26" s="16">
+        <v>0</v>
+      </c>
       <c r="W26"/>
       <c r="X26"/>
-    </row>
-    <row r="27" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="Y26"/>
+    </row>
+    <row r="27" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A27" s="13">
         <v>26</v>
       </c>
@@ -14074,17 +14183,21 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="T27" s="37">
-        <v>0</v>
-      </c>
-      <c r="U27" s="16">
-        <v>0</v>
-      </c>
-      <c r="V27"/>
+      <c r="T27" s="106">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
+      <c r="U27" s="37">
+        <v>0</v>
+      </c>
+      <c r="V27" s="16">
+        <v>0</v>
+      </c>
       <c r="W27"/>
       <c r="X27"/>
-    </row>
-    <row r="28" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="Y27"/>
+    </row>
+    <row r="28" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A28" s="13">
         <v>27</v>
       </c>
@@ -14140,17 +14253,21 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="T28" s="37">
-        <v>0</v>
-      </c>
-      <c r="U28" s="16">
-        <v>0</v>
-      </c>
-      <c r="V28"/>
+      <c r="T28" s="106">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
+      <c r="U28" s="37">
+        <v>0</v>
+      </c>
+      <c r="V28" s="16">
+        <v>0</v>
+      </c>
       <c r="W28"/>
       <c r="X28"/>
-    </row>
-    <row r="29" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="Y28"/>
+    </row>
+    <row r="29" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A29" s="13">
         <v>28</v>
       </c>
@@ -14206,17 +14323,21 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="T29" s="37">
-        <v>0</v>
-      </c>
-      <c r="U29" s="16">
-        <v>0</v>
-      </c>
-      <c r="V29"/>
+      <c r="T29" s="106">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="U29" s="37">
+        <v>0</v>
+      </c>
+      <c r="V29" s="16">
+        <v>0</v>
+      </c>
       <c r="W29"/>
       <c r="X29"/>
-    </row>
-    <row r="30" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="Y29"/>
+    </row>
+    <row r="30" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A30" s="23">
         <v>29</v>
       </c>
@@ -14272,17 +14393,21 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="T30" s="37">
-        <v>0</v>
-      </c>
-      <c r="U30" s="16">
-        <v>0</v>
-      </c>
-      <c r="V30"/>
+      <c r="T30" s="106">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="U30" s="37">
+        <v>0</v>
+      </c>
+      <c r="V30" s="16">
+        <v>0</v>
+      </c>
       <c r="W30"/>
       <c r="X30"/>
-    </row>
-    <row r="31" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="Y30"/>
+    </row>
+    <row r="31" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A31" s="13">
         <v>30</v>
       </c>
@@ -14338,17 +14463,21 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="T31" s="37">
-        <v>0</v>
-      </c>
-      <c r="U31" s="16">
-        <v>1</v>
-      </c>
-      <c r="V31"/>
+      <c r="T31" s="106">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="U31" s="37">
+        <v>0</v>
+      </c>
+      <c r="V31" s="16">
+        <v>1</v>
+      </c>
       <c r="W31"/>
       <c r="X31"/>
-    </row>
-    <row r="32" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="Y31"/>
+    </row>
+    <row r="32" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A32" s="23">
         <v>31</v>
       </c>
@@ -14404,17 +14533,21 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="T32" s="37">
-        <v>0</v>
-      </c>
-      <c r="U32" s="16">
-        <v>0</v>
-      </c>
-      <c r="V32"/>
+      <c r="T32" s="106">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="U32" s="37">
+        <v>0</v>
+      </c>
+      <c r="V32" s="16">
+        <v>0</v>
+      </c>
       <c r="W32"/>
       <c r="X32"/>
-    </row>
-    <row r="33" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="Y32"/>
+    </row>
+    <row r="33" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A33" s="13">
         <v>32</v>
       </c>
@@ -14470,17 +14603,21 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="T33" s="37">
-        <v>0</v>
-      </c>
-      <c r="U33" s="16">
-        <v>0</v>
-      </c>
-      <c r="V33"/>
+      <c r="T33" s="106">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="U33" s="37">
+        <v>0</v>
+      </c>
+      <c r="V33" s="16">
+        <v>0</v>
+      </c>
       <c r="W33"/>
       <c r="X33"/>
-    </row>
-    <row r="34" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="Y33"/>
+    </row>
+    <row r="34" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A34" s="13">
         <v>33</v>
       </c>
@@ -14536,17 +14673,21 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="T34" s="37">
-        <v>0</v>
-      </c>
-      <c r="U34" s="16">
-        <v>0</v>
-      </c>
-      <c r="V34"/>
+      <c r="T34" s="106">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="U34" s="37">
+        <v>0</v>
+      </c>
+      <c r="V34" s="16">
+        <v>0</v>
+      </c>
       <c r="W34"/>
       <c r="X34"/>
-    </row>
-    <row r="35" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="Y34"/>
+    </row>
+    <row r="35" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A35" s="13">
         <v>34</v>
       </c>
@@ -14602,17 +14743,21 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="T35" s="37">
-        <v>0</v>
-      </c>
-      <c r="U35" s="16">
-        <v>0</v>
-      </c>
-      <c r="V35"/>
+      <c r="T35" s="106">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="U35" s="37">
+        <v>0</v>
+      </c>
+      <c r="V35" s="16">
+        <v>0</v>
+      </c>
       <c r="W35"/>
       <c r="X35"/>
-    </row>
-    <row r="36" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="Y35"/>
+    </row>
+    <row r="36" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A36" s="13">
         <v>35</v>
       </c>
@@ -14668,17 +14813,21 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="T36" s="37">
-        <v>0</v>
-      </c>
-      <c r="U36" s="16">
-        <v>0</v>
-      </c>
-      <c r="V36"/>
+      <c r="T36" s="106">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="U36" s="37">
+        <v>0</v>
+      </c>
+      <c r="V36" s="16">
+        <v>0</v>
+      </c>
       <c r="W36"/>
       <c r="X36"/>
-    </row>
-    <row r="37" spans="1:24" ht="30" x14ac:dyDescent="0.25">
+      <c r="Y36"/>
+    </row>
+    <row r="37" spans="1:25" ht="30" x14ac:dyDescent="0.25">
       <c r="A37" s="13">
         <v>36</v>
       </c>
@@ -14734,17 +14883,21 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="T37" s="37">
-        <v>0</v>
-      </c>
-      <c r="U37" s="16">
-        <v>0</v>
-      </c>
-      <c r="V37"/>
+      <c r="T37" s="106">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="U37" s="37">
+        <v>0</v>
+      </c>
+      <c r="V37" s="16">
+        <v>0</v>
+      </c>
       <c r="W37"/>
       <c r="X37"/>
-    </row>
-    <row r="38" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="Y37"/>
+    </row>
+    <row r="38" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A38" s="13">
         <v>37</v>
       </c>
@@ -14800,17 +14953,21 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="T38" s="37">
-        <v>0</v>
-      </c>
-      <c r="U38" s="16">
-        <v>0</v>
-      </c>
-      <c r="V38"/>
+      <c r="T38" s="106">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="U38" s="37">
+        <v>0</v>
+      </c>
+      <c r="V38" s="16">
+        <v>0</v>
+      </c>
       <c r="W38"/>
       <c r="X38"/>
-    </row>
-    <row r="39" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="Y38"/>
+    </row>
+    <row r="39" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A39" s="13">
         <v>38</v>
       </c>
@@ -14866,17 +15023,21 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="T39" s="37">
-        <v>0</v>
-      </c>
-      <c r="U39" s="16">
-        <v>0</v>
-      </c>
-      <c r="V39"/>
+      <c r="T39" s="106">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="U39" s="37">
+        <v>0</v>
+      </c>
+      <c r="V39" s="16">
+        <v>0</v>
+      </c>
       <c r="W39"/>
       <c r="X39"/>
-    </row>
-    <row r="40" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="Y39"/>
+    </row>
+    <row r="40" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A40" s="13">
         <v>39</v>
       </c>
@@ -14932,17 +15093,21 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="T40" s="37">
-        <v>0</v>
-      </c>
-      <c r="U40" s="16">
-        <v>0</v>
-      </c>
-      <c r="V40"/>
+      <c r="T40" s="106">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="U40" s="37">
+        <v>0</v>
+      </c>
+      <c r="V40" s="16">
+        <v>0</v>
+      </c>
       <c r="W40"/>
       <c r="X40"/>
-    </row>
-    <row r="41" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="Y40"/>
+    </row>
+    <row r="41" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A41" s="23">
         <v>40</v>
       </c>
@@ -14998,17 +15163,21 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="T41" s="37">
-        <v>0</v>
-      </c>
-      <c r="U41" s="16">
-        <v>0</v>
-      </c>
-      <c r="V41"/>
+      <c r="T41" s="106">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="U41" s="37">
+        <v>0</v>
+      </c>
+      <c r="V41" s="16">
+        <v>0</v>
+      </c>
       <c r="W41"/>
       <c r="X41"/>
-    </row>
-    <row r="42" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="Y41"/>
+    </row>
+    <row r="42" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A42" s="13">
         <v>41</v>
       </c>
@@ -15064,17 +15233,21 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="T42" s="37">
-        <v>0</v>
-      </c>
-      <c r="U42" s="16">
-        <v>0</v>
-      </c>
-      <c r="V42"/>
+      <c r="T42" s="106">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="U42" s="37">
+        <v>0</v>
+      </c>
+      <c r="V42" s="16">
+        <v>0</v>
+      </c>
       <c r="W42"/>
       <c r="X42"/>
-    </row>
-    <row r="43" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="Y42"/>
+    </row>
+    <row r="43" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A43" s="13">
         <v>1</v>
       </c>
@@ -15130,17 +15303,21 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="T43" s="37">
-        <v>1</v>
-      </c>
-      <c r="U43" s="16">
-        <v>0</v>
-      </c>
-      <c r="V43"/>
+      <c r="T43" s="106">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
+      <c r="U43" s="37">
+        <v>1</v>
+      </c>
+      <c r="V43" s="16">
+        <v>0</v>
+      </c>
       <c r="W43"/>
       <c r="X43"/>
-    </row>
-    <row r="44" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="Y43"/>
+    </row>
+    <row r="44" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A44" s="13">
         <v>43</v>
       </c>
@@ -15196,17 +15373,21 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="T44" s="37">
-        <v>0</v>
-      </c>
-      <c r="U44" s="16">
-        <v>0</v>
-      </c>
-      <c r="V44"/>
+      <c r="T44" s="106">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="U44" s="37">
+        <v>0</v>
+      </c>
+      <c r="V44" s="16">
+        <v>0</v>
+      </c>
       <c r="W44"/>
       <c r="X44"/>
-    </row>
-    <row r="45" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="Y44"/>
+    </row>
+    <row r="45" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A45" s="13">
         <v>44</v>
       </c>
@@ -15262,17 +15443,21 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="T45" s="37">
-        <v>0</v>
-      </c>
-      <c r="U45" s="16">
-        <v>0</v>
-      </c>
-      <c r="V45"/>
+      <c r="T45" s="106">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="U45" s="37">
+        <v>0</v>
+      </c>
+      <c r="V45" s="16">
+        <v>0</v>
+      </c>
       <c r="W45"/>
       <c r="X45"/>
-    </row>
-    <row r="46" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="Y45"/>
+    </row>
+    <row r="46" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A46" s="13">
         <v>45</v>
       </c>
@@ -15328,17 +15513,21 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="T46" s="37">
-        <v>0</v>
-      </c>
-      <c r="U46" s="16">
-        <v>0</v>
-      </c>
-      <c r="V46"/>
+      <c r="T46" s="106">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="U46" s="37">
+        <v>0</v>
+      </c>
+      <c r="V46" s="16">
+        <v>0</v>
+      </c>
       <c r="W46"/>
       <c r="X46"/>
-    </row>
-    <row r="47" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="Y46"/>
+    </row>
+    <row r="47" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A47" s="13">
         <v>46</v>
       </c>
@@ -15394,17 +15583,21 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="T47" s="37">
-        <v>0</v>
-      </c>
-      <c r="U47" s="16">
-        <v>0</v>
-      </c>
-      <c r="V47"/>
+      <c r="T47" s="106">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="U47" s="37">
+        <v>0</v>
+      </c>
+      <c r="V47" s="16">
+        <v>0</v>
+      </c>
       <c r="W47"/>
       <c r="X47"/>
-    </row>
-    <row r="48" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="Y47"/>
+    </row>
+    <row r="48" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A48" s="13">
         <v>47</v>
       </c>
@@ -15460,17 +15653,21 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="T48" s="37">
-        <v>1</v>
-      </c>
-      <c r="U48" s="16">
-        <v>0</v>
-      </c>
-      <c r="V48"/>
+      <c r="T48" s="106">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
+      <c r="U48" s="37">
+        <v>1</v>
+      </c>
+      <c r="V48" s="16">
+        <v>0</v>
+      </c>
       <c r="W48"/>
       <c r="X48"/>
-    </row>
-    <row r="49" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="Y48"/>
+    </row>
+    <row r="49" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A49" s="13">
         <v>48</v>
       </c>
@@ -15526,17 +15723,21 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="T49" s="37">
-        <v>0</v>
-      </c>
-      <c r="U49" s="16">
-        <v>0</v>
-      </c>
-      <c r="V49"/>
+      <c r="T49" s="106">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
+      <c r="U49" s="37">
+        <v>0</v>
+      </c>
+      <c r="V49" s="16">
+        <v>0</v>
+      </c>
       <c r="W49"/>
       <c r="X49"/>
-    </row>
-    <row r="50" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="Y49"/>
+    </row>
+    <row r="50" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A50" s="13">
         <v>49</v>
       </c>
@@ -15592,17 +15793,21 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="T50" s="37">
-        <v>0</v>
-      </c>
-      <c r="U50" s="16">
-        <v>0</v>
-      </c>
-      <c r="V50"/>
+      <c r="T50" s="106">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="U50" s="37">
+        <v>0</v>
+      </c>
+      <c r="V50" s="16">
+        <v>0</v>
+      </c>
       <c r="W50"/>
       <c r="X50"/>
-    </row>
-    <row r="51" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="Y50"/>
+    </row>
+    <row r="51" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A51" s="13">
         <v>50</v>
       </c>
@@ -15658,17 +15863,21 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="T51" s="37">
-        <v>0</v>
-      </c>
-      <c r="U51" s="16">
-        <v>0</v>
-      </c>
-      <c r="V51"/>
+      <c r="T51" s="106">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="U51" s="37">
+        <v>0</v>
+      </c>
+      <c r="V51" s="16">
+        <v>0</v>
+      </c>
       <c r="W51"/>
       <c r="X51"/>
-    </row>
-    <row r="52" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="Y51"/>
+    </row>
+    <row r="52" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A52" s="27">
         <v>51</v>
       </c>
@@ -15724,17 +15933,21 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="T52" s="37">
-        <v>0</v>
-      </c>
-      <c r="U52" s="16">
-        <v>0</v>
-      </c>
-      <c r="V52"/>
+      <c r="T52" s="106">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
+      <c r="U52" s="37">
+        <v>0</v>
+      </c>
+      <c r="V52" s="16">
+        <v>0</v>
+      </c>
       <c r="W52"/>
       <c r="X52"/>
-    </row>
-    <row r="53" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="Y52"/>
+    </row>
+    <row r="53" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A53" s="13">
         <v>52</v>
       </c>
@@ -15790,17 +16003,21 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="T53" s="37">
-        <v>0</v>
-      </c>
-      <c r="U53" s="16">
-        <v>0</v>
-      </c>
-      <c r="V53"/>
+      <c r="T53" s="106">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="U53" s="37">
+        <v>0</v>
+      </c>
+      <c r="V53" s="16">
+        <v>0</v>
+      </c>
       <c r="W53"/>
       <c r="X53"/>
-    </row>
-    <row r="54" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="Y53"/>
+    </row>
+    <row r="54" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A54" s="13">
         <v>53</v>
       </c>
@@ -15856,17 +16073,21 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="T54" s="37">
-        <v>0</v>
-      </c>
-      <c r="U54" s="16">
-        <v>0</v>
-      </c>
-      <c r="V54"/>
+      <c r="T54" s="106">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="U54" s="37">
+        <v>0</v>
+      </c>
+      <c r="V54" s="16">
+        <v>0</v>
+      </c>
       <c r="W54"/>
       <c r="X54"/>
-    </row>
-    <row r="55" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="Y54"/>
+    </row>
+    <row r="55" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A55" s="13">
         <v>54</v>
       </c>
@@ -15922,17 +16143,21 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="T55" s="37">
-        <v>0</v>
-      </c>
-      <c r="U55" s="16">
-        <v>0</v>
-      </c>
-      <c r="V55"/>
+      <c r="T55" s="106">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="U55" s="37">
+        <v>0</v>
+      </c>
+      <c r="V55" s="16">
+        <v>0</v>
+      </c>
       <c r="W55"/>
       <c r="X55"/>
-    </row>
-    <row r="56" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="Y55"/>
+    </row>
+    <row r="56" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A56" s="13">
         <v>55</v>
       </c>
@@ -15988,17 +16213,21 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="T56" s="37">
-        <v>0</v>
-      </c>
-      <c r="U56" s="16">
-        <v>0</v>
-      </c>
-      <c r="V56"/>
+      <c r="T56" s="106">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="U56" s="37">
+        <v>0</v>
+      </c>
+      <c r="V56" s="16">
+        <v>0</v>
+      </c>
       <c r="W56"/>
       <c r="X56"/>
-    </row>
-    <row r="57" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="Y56"/>
+    </row>
+    <row r="57" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A57" s="13">
         <v>56</v>
       </c>
@@ -16054,17 +16283,21 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="T57" s="37">
-        <v>1</v>
-      </c>
-      <c r="U57" s="16">
-        <v>0</v>
-      </c>
-      <c r="V57"/>
+      <c r="T57" s="106">
+        <f t="shared" si="1"/>
+        <v>6</v>
+      </c>
+      <c r="U57" s="37">
+        <v>1</v>
+      </c>
+      <c r="V57" s="16">
+        <v>0</v>
+      </c>
       <c r="W57"/>
       <c r="X57"/>
-    </row>
-    <row r="58" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="Y57"/>
+    </row>
+    <row r="58" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A58" s="13">
         <v>57</v>
       </c>
@@ -16120,17 +16353,21 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="T58" s="37">
-        <v>1</v>
-      </c>
-      <c r="U58" s="16">
-        <v>0</v>
-      </c>
-      <c r="V58"/>
+      <c r="T58" s="106">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
+      <c r="U58" s="37">
+        <v>1</v>
+      </c>
+      <c r="V58" s="16">
+        <v>0</v>
+      </c>
       <c r="W58"/>
       <c r="X58"/>
-    </row>
-    <row r="59" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="Y58"/>
+    </row>
+    <row r="59" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A59" s="23">
         <v>58</v>
       </c>
@@ -16186,17 +16423,21 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="T59" s="37">
-        <v>0</v>
-      </c>
-      <c r="U59" s="16">
-        <v>0</v>
-      </c>
-      <c r="V59"/>
+      <c r="T59" s="106">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="U59" s="37">
+        <v>0</v>
+      </c>
+      <c r="V59" s="16">
+        <v>0</v>
+      </c>
       <c r="W59"/>
       <c r="X59"/>
-    </row>
-    <row r="60" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="Y59"/>
+    </row>
+    <row r="60" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A60" s="13">
         <v>59</v>
       </c>
@@ -16252,17 +16493,21 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="T60" s="37">
-        <v>0</v>
-      </c>
-      <c r="U60" s="16">
-        <v>0</v>
-      </c>
-      <c r="V60"/>
+      <c r="T60" s="106">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="U60" s="37">
+        <v>0</v>
+      </c>
+      <c r="V60" s="16">
+        <v>0</v>
+      </c>
       <c r="W60"/>
       <c r="X60"/>
-    </row>
-    <row r="61" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="Y60"/>
+    </row>
+    <row r="61" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A61" s="13">
         <v>60</v>
       </c>
@@ -16318,17 +16563,21 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="T61" s="37">
-        <v>0</v>
-      </c>
-      <c r="U61" s="16">
-        <v>0</v>
-      </c>
-      <c r="V61"/>
+      <c r="T61" s="106">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="U61" s="37">
+        <v>0</v>
+      </c>
+      <c r="V61" s="16">
+        <v>0</v>
+      </c>
       <c r="W61"/>
       <c r="X61"/>
-    </row>
-    <row r="62" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="Y61"/>
+    </row>
+    <row r="62" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A62" s="13">
         <v>61</v>
       </c>
@@ -16384,17 +16633,21 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="T62" s="37">
-        <v>0</v>
-      </c>
-      <c r="U62" s="16">
-        <v>0</v>
-      </c>
-      <c r="V62"/>
+      <c r="T62" s="106">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="U62" s="37">
+        <v>0</v>
+      </c>
+      <c r="V62" s="16">
+        <v>0</v>
+      </c>
       <c r="W62"/>
       <c r="X62"/>
-    </row>
-    <row r="63" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="Y62"/>
+    </row>
+    <row r="63" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A63" s="13">
         <v>62</v>
       </c>
@@ -16450,17 +16703,21 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="T63" s="37">
-        <v>0</v>
-      </c>
-      <c r="U63" s="16">
-        <v>0</v>
-      </c>
-      <c r="V63"/>
+      <c r="T63" s="106">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="U63" s="37">
+        <v>0</v>
+      </c>
+      <c r="V63" s="16">
+        <v>0</v>
+      </c>
       <c r="W63"/>
       <c r="X63"/>
-    </row>
-    <row r="64" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="Y63"/>
+    </row>
+    <row r="64" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A64" s="13">
         <v>63</v>
       </c>
@@ -16516,17 +16773,21 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="T64" s="37">
-        <v>0</v>
-      </c>
-      <c r="U64" s="16">
-        <v>0</v>
-      </c>
-      <c r="V64"/>
+      <c r="T64" s="106">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="U64" s="37">
+        <v>0</v>
+      </c>
+      <c r="V64" s="16">
+        <v>0</v>
+      </c>
       <c r="W64"/>
       <c r="X64"/>
-    </row>
-    <row r="65" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="Y64"/>
+    </row>
+    <row r="65" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A65" s="13">
         <v>64</v>
       </c>
@@ -16582,17 +16843,21 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="T65" s="37">
-        <v>0</v>
-      </c>
-      <c r="U65" s="16">
-        <v>0</v>
-      </c>
-      <c r="V65"/>
+      <c r="T65" s="106">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="U65" s="37">
+        <v>0</v>
+      </c>
+      <c r="V65" s="16">
+        <v>0</v>
+      </c>
       <c r="W65"/>
       <c r="X65"/>
-    </row>
-    <row r="66" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="Y65"/>
+    </row>
+    <row r="66" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A66" s="13">
         <v>65</v>
       </c>
@@ -16648,17 +16913,21 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="T66" s="37">
-        <v>0</v>
-      </c>
-      <c r="U66" s="16">
-        <v>0</v>
-      </c>
-      <c r="V66"/>
+      <c r="T66" s="106">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
+      <c r="U66" s="37">
+        <v>0</v>
+      </c>
+      <c r="V66" s="16">
+        <v>0</v>
+      </c>
       <c r="W66"/>
       <c r="X66"/>
-    </row>
-    <row r="67" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="Y66"/>
+    </row>
+    <row r="67" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A67" s="23">
         <v>66</v>
       </c>
@@ -16711,20 +16980,24 @@
         <v>0</v>
       </c>
       <c r="R67" s="62">
-        <f t="shared" ref="R67:R124" si="1">SUM(T67:U67)</f>
-        <v>0</v>
-      </c>
-      <c r="T67" s="37">
-        <v>0</v>
-      </c>
-      <c r="U67" s="16">
-        <v>0</v>
-      </c>
-      <c r="V67"/>
+        <f t="shared" ref="R67:R124" si="2">SUM(U67:V67)</f>
+        <v>0</v>
+      </c>
+      <c r="T67" s="106">
+        <f t="shared" ref="T67:T124" si="3">SUM(H67:R67)</f>
+        <v>2</v>
+      </c>
+      <c r="U67" s="37">
+        <v>0</v>
+      </c>
+      <c r="V67" s="16">
+        <v>0</v>
+      </c>
       <c r="W67"/>
       <c r="X67"/>
-    </row>
-    <row r="68" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="Y67"/>
+    </row>
+    <row r="68" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A68" s="13">
         <v>67</v>
       </c>
@@ -16777,20 +17050,24 @@
         <v>0</v>
       </c>
       <c r="R68" s="62">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="T68" s="37">
-        <v>0</v>
-      </c>
-      <c r="U68" s="16">
-        <v>0</v>
-      </c>
-      <c r="V68"/>
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="T68" s="106">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+      <c r="U68" s="37">
+        <v>0</v>
+      </c>
+      <c r="V68" s="16">
+        <v>0</v>
+      </c>
       <c r="W68"/>
       <c r="X68"/>
-    </row>
-    <row r="69" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="Y68"/>
+    </row>
+    <row r="69" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A69" s="13">
         <v>68</v>
       </c>
@@ -16843,20 +17120,24 @@
         <v>0</v>
       </c>
       <c r="R69" s="62">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="T69" s="37">
-        <v>0</v>
-      </c>
-      <c r="U69" s="16">
-        <v>0</v>
-      </c>
-      <c r="V69"/>
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="T69" s="106">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+      <c r="U69" s="37">
+        <v>0</v>
+      </c>
+      <c r="V69" s="16">
+        <v>0</v>
+      </c>
       <c r="W69"/>
       <c r="X69"/>
-    </row>
-    <row r="70" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="Y69"/>
+    </row>
+    <row r="70" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A70" s="23">
         <v>69</v>
       </c>
@@ -16909,20 +17190,24 @@
         <v>0</v>
       </c>
       <c r="R70" s="62">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="T70" s="37">
-        <v>0</v>
-      </c>
-      <c r="U70" s="16">
-        <v>0</v>
-      </c>
-      <c r="V70"/>
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="T70" s="106">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+      <c r="U70" s="37">
+        <v>0</v>
+      </c>
+      <c r="V70" s="16">
+        <v>0</v>
+      </c>
       <c r="W70"/>
       <c r="X70"/>
-    </row>
-    <row r="71" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="Y70"/>
+    </row>
+    <row r="71" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A71" s="13">
         <v>70</v>
       </c>
@@ -16975,20 +17260,24 @@
         <v>0</v>
       </c>
       <c r="R71" s="62">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="T71" s="37">
-        <v>0</v>
-      </c>
-      <c r="U71" s="16">
-        <v>0</v>
-      </c>
-      <c r="V71"/>
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="T71" s="106">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+      <c r="U71" s="37">
+        <v>0</v>
+      </c>
+      <c r="V71" s="16">
+        <v>0</v>
+      </c>
       <c r="W71"/>
       <c r="X71"/>
-    </row>
-    <row r="72" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="Y71"/>
+    </row>
+    <row r="72" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A72" s="13">
         <v>71</v>
       </c>
@@ -17041,20 +17330,24 @@
         <v>0</v>
       </c>
       <c r="R72" s="62">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="T72" s="37">
-        <v>0</v>
-      </c>
-      <c r="U72" s="16">
-        <v>1</v>
-      </c>
-      <c r="V72"/>
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="T72" s="106">
+        <f t="shared" si="3"/>
+        <v>3</v>
+      </c>
+      <c r="U72" s="37">
+        <v>0</v>
+      </c>
+      <c r="V72" s="16">
+        <v>1</v>
+      </c>
       <c r="W72"/>
       <c r="X72"/>
-    </row>
-    <row r="73" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="Y72"/>
+    </row>
+    <row r="73" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A73" s="13">
         <v>72</v>
       </c>
@@ -17107,20 +17400,24 @@
         <v>0</v>
       </c>
       <c r="R73" s="62">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="T73" s="37">
-        <v>0</v>
-      </c>
-      <c r="U73" s="16">
-        <v>0</v>
-      </c>
-      <c r="V73"/>
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="T73" s="106">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+      <c r="U73" s="37">
+        <v>0</v>
+      </c>
+      <c r="V73" s="16">
+        <v>0</v>
+      </c>
       <c r="W73"/>
       <c r="X73"/>
-    </row>
-    <row r="74" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="Y73"/>
+    </row>
+    <row r="74" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A74" s="13">
         <v>73</v>
       </c>
@@ -17173,20 +17470,24 @@
         <v>0</v>
       </c>
       <c r="R74" s="62">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="T74" s="37">
-        <v>0</v>
-      </c>
-      <c r="U74" s="16">
-        <v>0</v>
-      </c>
-      <c r="V74"/>
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="T74" s="106">
+        <f t="shared" si="3"/>
+        <v>4</v>
+      </c>
+      <c r="U74" s="37">
+        <v>0</v>
+      </c>
+      <c r="V74" s="16">
+        <v>0</v>
+      </c>
       <c r="W74"/>
       <c r="X74"/>
-    </row>
-    <row r="75" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="Y74"/>
+    </row>
+    <row r="75" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A75" s="13">
         <v>74</v>
       </c>
@@ -17239,20 +17540,24 @@
         <v>0</v>
       </c>
       <c r="R75" s="62">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="T75" s="37">
-        <v>0</v>
-      </c>
-      <c r="U75" s="16">
-        <v>0</v>
-      </c>
-      <c r="V75"/>
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="T75" s="106">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+      <c r="U75" s="37">
+        <v>0</v>
+      </c>
+      <c r="V75" s="16">
+        <v>0</v>
+      </c>
       <c r="W75"/>
       <c r="X75"/>
-    </row>
-    <row r="76" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="Y75"/>
+    </row>
+    <row r="76" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A76" s="23">
         <v>75</v>
       </c>
@@ -17305,20 +17610,24 @@
         <v>0</v>
       </c>
       <c r="R76" s="62">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="T76" s="37">
-        <v>0</v>
-      </c>
-      <c r="U76" s="16">
-        <v>0</v>
-      </c>
-      <c r="V76"/>
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="T76" s="106">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+      <c r="U76" s="37">
+        <v>0</v>
+      </c>
+      <c r="V76" s="16">
+        <v>0</v>
+      </c>
       <c r="W76"/>
       <c r="X76"/>
-    </row>
-    <row r="77" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="Y76"/>
+    </row>
+    <row r="77" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A77" s="13">
         <v>76</v>
       </c>
@@ -17371,20 +17680,24 @@
         <v>0</v>
       </c>
       <c r="R77" s="62">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="T77" s="37">
-        <v>0</v>
-      </c>
-      <c r="U77" s="16">
-        <v>0</v>
-      </c>
-      <c r="V77"/>
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="T77" s="106">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="U77" s="37">
+        <v>0</v>
+      </c>
+      <c r="V77" s="16">
+        <v>0</v>
+      </c>
       <c r="W77"/>
       <c r="X77"/>
-    </row>
-    <row r="78" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="Y77"/>
+    </row>
+    <row r="78" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A78" s="13">
         <v>77</v>
       </c>
@@ -17437,20 +17750,24 @@
         <v>0</v>
       </c>
       <c r="R78" s="62">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="T78" s="37">
-        <v>0</v>
-      </c>
-      <c r="U78" s="16">
-        <v>0</v>
-      </c>
-      <c r="V78"/>
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="T78" s="106">
+        <f t="shared" si="3"/>
+        <v>3</v>
+      </c>
+      <c r="U78" s="37">
+        <v>0</v>
+      </c>
+      <c r="V78" s="16">
+        <v>0</v>
+      </c>
       <c r="W78"/>
       <c r="X78"/>
-    </row>
-    <row r="79" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="Y78"/>
+    </row>
+    <row r="79" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A79" s="13">
         <v>78</v>
       </c>
@@ -17503,20 +17820,24 @@
         <v>0</v>
       </c>
       <c r="R79" s="62">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="T79" s="37">
-        <v>0</v>
-      </c>
-      <c r="U79" s="16">
-        <v>0</v>
-      </c>
-      <c r="V79"/>
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="T79" s="106">
+        <f t="shared" si="3"/>
+        <v>3</v>
+      </c>
+      <c r="U79" s="37">
+        <v>0</v>
+      </c>
+      <c r="V79" s="16">
+        <v>0</v>
+      </c>
       <c r="W79"/>
       <c r="X79"/>
-    </row>
-    <row r="80" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="Y79"/>
+    </row>
+    <row r="80" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A80" s="13">
         <v>79</v>
       </c>
@@ -17569,20 +17890,24 @@
         <v>0</v>
       </c>
       <c r="R80" s="62">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="T80" s="37">
-        <v>0</v>
-      </c>
-      <c r="U80" s="16">
-        <v>0</v>
-      </c>
-      <c r="V80"/>
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="T80" s="106">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+      <c r="U80" s="37">
+        <v>0</v>
+      </c>
+      <c r="V80" s="16">
+        <v>0</v>
+      </c>
       <c r="W80"/>
       <c r="X80"/>
-    </row>
-    <row r="81" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="Y80"/>
+    </row>
+    <row r="81" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A81" s="13">
         <v>80</v>
       </c>
@@ -17635,25 +17960,29 @@
         <v>0</v>
       </c>
       <c r="R81" s="62">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="T81" s="37">
-        <v>0</v>
-      </c>
-      <c r="U81" s="16">
-        <v>0</v>
-      </c>
-      <c r="V81"/>
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="T81" s="106">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+      <c r="U81" s="37">
+        <v>0</v>
+      </c>
+      <c r="V81" s="16">
+        <v>0</v>
+      </c>
       <c r="W81"/>
       <c r="X81"/>
-    </row>
-    <row r="82" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="Y81"/>
+    </row>
+    <row r="82" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A82" s="13">
         <v>81</v>
       </c>
       <c r="B82" s="13" t="s">
-        <v>2</v>
+        <v>748</v>
       </c>
       <c r="C82" s="13">
         <v>2017</v>
@@ -17701,25 +18030,29 @@
         <v>0</v>
       </c>
       <c r="R82" s="62">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="T82" s="37">
-        <v>0</v>
-      </c>
-      <c r="U82" s="16">
-        <v>0</v>
-      </c>
-      <c r="V82"/>
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="T82" s="106">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="U82" s="37">
+        <v>0</v>
+      </c>
+      <c r="V82" s="16">
+        <v>0</v>
+      </c>
       <c r="W82"/>
       <c r="X82"/>
-    </row>
-    <row r="83" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="Y82"/>
+    </row>
+    <row r="83" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A83" s="13">
         <v>82</v>
       </c>
       <c r="B83" s="13" t="s">
-        <v>2</v>
+        <v>749</v>
       </c>
       <c r="C83" s="13">
         <v>2017</v>
@@ -17767,20 +18100,24 @@
         <v>0</v>
       </c>
       <c r="R83" s="62">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="T83" s="37">
-        <v>0</v>
-      </c>
-      <c r="U83" s="16">
-        <v>0</v>
-      </c>
-      <c r="V83"/>
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="T83" s="106">
+        <f t="shared" si="3"/>
+        <v>3</v>
+      </c>
+      <c r="U83" s="37">
+        <v>0</v>
+      </c>
+      <c r="V83" s="16">
+        <v>0</v>
+      </c>
       <c r="W83"/>
       <c r="X83"/>
-    </row>
-    <row r="84" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="Y83"/>
+    </row>
+    <row r="84" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A84" s="27">
         <v>83</v>
       </c>
@@ -17833,20 +18170,24 @@
         <v>0</v>
       </c>
       <c r="R84" s="62">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="T84" s="37">
-        <v>0</v>
-      </c>
-      <c r="U84" s="16">
-        <v>0</v>
-      </c>
-      <c r="V84"/>
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="T84" s="106">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="U84" s="37">
+        <v>0</v>
+      </c>
+      <c r="V84" s="16">
+        <v>0</v>
+      </c>
       <c r="W84"/>
       <c r="X84"/>
-    </row>
-    <row r="85" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="Y84"/>
+    </row>
+    <row r="85" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A85" s="27">
         <v>84</v>
       </c>
@@ -17899,20 +18240,24 @@
         <v>0</v>
       </c>
       <c r="R85" s="62">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="T85" s="37">
-        <v>0</v>
-      </c>
-      <c r="U85" s="16">
-        <v>0</v>
-      </c>
-      <c r="V85"/>
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="T85" s="106">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+      <c r="U85" s="37">
+        <v>0</v>
+      </c>
+      <c r="V85" s="16">
+        <v>0</v>
+      </c>
       <c r="W85"/>
       <c r="X85"/>
-    </row>
-    <row r="86" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="Y85"/>
+    </row>
+    <row r="86" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A86" s="13">
         <v>85</v>
       </c>
@@ -17965,20 +18310,24 @@
         <v>0</v>
       </c>
       <c r="R86" s="62">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="T86" s="37">
-        <v>0</v>
-      </c>
-      <c r="U86" s="16">
-        <v>0</v>
-      </c>
-      <c r="V86"/>
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="T86" s="106">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+      <c r="U86" s="37">
+        <v>0</v>
+      </c>
+      <c r="V86" s="16">
+        <v>0</v>
+      </c>
       <c r="W86"/>
       <c r="X86"/>
-    </row>
-    <row r="87" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="Y86"/>
+    </row>
+    <row r="87" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A87" s="13">
         <v>86</v>
       </c>
@@ -18031,20 +18380,24 @@
         <v>0</v>
       </c>
       <c r="R87" s="62">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="T87" s="37">
-        <v>0</v>
-      </c>
-      <c r="U87" s="16">
-        <v>0</v>
-      </c>
-      <c r="V87"/>
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="T87" s="106">
+        <f t="shared" si="3"/>
+        <v>3</v>
+      </c>
+      <c r="U87" s="37">
+        <v>0</v>
+      </c>
+      <c r="V87" s="16">
+        <v>0</v>
+      </c>
       <c r="W87"/>
       <c r="X87"/>
-    </row>
-    <row r="88" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="Y87"/>
+    </row>
+    <row r="88" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A88" s="13">
         <v>87</v>
       </c>
@@ -18097,20 +18450,24 @@
         <v>0</v>
       </c>
       <c r="R88" s="62">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="T88" s="37">
-        <v>0</v>
-      </c>
-      <c r="U88" s="16">
-        <v>0</v>
-      </c>
-      <c r="V88"/>
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="T88" s="106">
+        <f t="shared" si="3"/>
+        <v>4</v>
+      </c>
+      <c r="U88" s="37">
+        <v>0</v>
+      </c>
+      <c r="V88" s="16">
+        <v>0</v>
+      </c>
       <c r="W88"/>
       <c r="X88"/>
-    </row>
-    <row r="89" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="Y88"/>
+    </row>
+    <row r="89" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A89" s="13">
         <v>88</v>
       </c>
@@ -18163,20 +18520,24 @@
         <v>0</v>
       </c>
       <c r="R89" s="62">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="T89" s="37">
-        <v>0</v>
-      </c>
-      <c r="U89" s="16">
-        <v>0</v>
-      </c>
-      <c r="V89"/>
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="T89" s="106">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="U89" s="37">
+        <v>0</v>
+      </c>
+      <c r="V89" s="16">
+        <v>0</v>
+      </c>
       <c r="W89"/>
       <c r="X89"/>
-    </row>
-    <row r="90" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="Y89"/>
+    </row>
+    <row r="90" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A90" s="13">
         <v>89</v>
       </c>
@@ -18229,20 +18590,24 @@
         <v>0</v>
       </c>
       <c r="R90" s="62">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="T90" s="37">
-        <v>0</v>
-      </c>
-      <c r="U90" s="16">
-        <v>0</v>
-      </c>
-      <c r="V90"/>
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="T90" s="106">
+        <f t="shared" si="3"/>
+        <v>3</v>
+      </c>
+      <c r="U90" s="37">
+        <v>0</v>
+      </c>
+      <c r="V90" s="16">
+        <v>0</v>
+      </c>
       <c r="W90"/>
       <c r="X90"/>
-    </row>
-    <row r="91" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="Y90"/>
+    </row>
+    <row r="91" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A91" s="13">
         <v>90</v>
       </c>
@@ -18295,20 +18660,24 @@
         <v>0</v>
       </c>
       <c r="R91" s="62">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="T91" s="37">
-        <v>0</v>
-      </c>
-      <c r="U91" s="16">
-        <v>0</v>
-      </c>
-      <c r="V91"/>
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="T91" s="106">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="U91" s="37">
+        <v>0</v>
+      </c>
+      <c r="V91" s="16">
+        <v>0</v>
+      </c>
       <c r="W91"/>
       <c r="X91"/>
-    </row>
-    <row r="92" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="Y91"/>
+    </row>
+    <row r="92" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A92" s="13">
         <v>91</v>
       </c>
@@ -18361,20 +18730,24 @@
         <v>0</v>
       </c>
       <c r="R92" s="62">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="T92" s="37">
-        <v>0</v>
-      </c>
-      <c r="U92" s="16">
-        <v>0</v>
-      </c>
-      <c r="V92"/>
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="T92" s="106">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+      <c r="U92" s="37">
+        <v>0</v>
+      </c>
+      <c r="V92" s="16">
+        <v>0</v>
+      </c>
       <c r="W92"/>
       <c r="X92"/>
-    </row>
-    <row r="93" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="Y92"/>
+    </row>
+    <row r="93" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A93" s="27">
         <v>92</v>
       </c>
@@ -18427,20 +18800,24 @@
         <v>0</v>
       </c>
       <c r="R93" s="62">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="T93" s="37">
-        <v>0</v>
-      </c>
-      <c r="U93" s="16">
-        <v>0</v>
-      </c>
-      <c r="V93"/>
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="T93" s="106">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+      <c r="U93" s="37">
+        <v>0</v>
+      </c>
+      <c r="V93" s="16">
+        <v>0</v>
+      </c>
       <c r="W93"/>
       <c r="X93"/>
-    </row>
-    <row r="94" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="Y93"/>
+    </row>
+    <row r="94" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A94" s="13">
         <v>93</v>
       </c>
@@ -18493,20 +18870,24 @@
         <v>0</v>
       </c>
       <c r="R94" s="62">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="T94" s="37">
-        <v>0</v>
-      </c>
-      <c r="U94" s="16">
-        <v>0</v>
-      </c>
-      <c r="V94"/>
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="T94" s="106">
+        <f t="shared" si="3"/>
+        <v>3</v>
+      </c>
+      <c r="U94" s="37">
+        <v>0</v>
+      </c>
+      <c r="V94" s="16">
+        <v>0</v>
+      </c>
       <c r="W94"/>
       <c r="X94"/>
-    </row>
-    <row r="95" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="Y94"/>
+    </row>
+    <row r="95" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A95" s="13">
         <v>94</v>
       </c>
@@ -18559,20 +18940,24 @@
         <v>0</v>
       </c>
       <c r="R95" s="62">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="T95" s="37">
-        <v>0</v>
-      </c>
-      <c r="U95" s="16">
-        <v>0</v>
-      </c>
-      <c r="V95"/>
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="T95" s="106">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="U95" s="37">
+        <v>0</v>
+      </c>
+      <c r="V95" s="16">
+        <v>0</v>
+      </c>
       <c r="W95"/>
       <c r="X95"/>
-    </row>
-    <row r="96" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="Y95"/>
+    </row>
+    <row r="96" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A96" s="13">
         <v>95</v>
       </c>
@@ -18625,20 +19010,24 @@
         <v>0</v>
       </c>
       <c r="R96" s="62">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="T96" s="37">
-        <v>0</v>
-      </c>
-      <c r="U96" s="16">
-        <v>0</v>
-      </c>
-      <c r="V96"/>
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="T96" s="106">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+      <c r="U96" s="37">
+        <v>0</v>
+      </c>
+      <c r="V96" s="16">
+        <v>0</v>
+      </c>
       <c r="W96"/>
       <c r="X96"/>
-    </row>
-    <row r="97" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="Y96"/>
+    </row>
+    <row r="97" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A97" s="13">
         <v>96</v>
       </c>
@@ -18691,20 +19080,24 @@
         <v>0</v>
       </c>
       <c r="R97" s="62">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="T97" s="37">
-        <v>0</v>
-      </c>
-      <c r="U97" s="16">
-        <v>0</v>
-      </c>
-      <c r="V97"/>
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="T97" s="106">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+      <c r="U97" s="37">
+        <v>0</v>
+      </c>
+      <c r="V97" s="16">
+        <v>0</v>
+      </c>
       <c r="W97"/>
       <c r="X97"/>
-    </row>
-    <row r="98" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="Y97"/>
+    </row>
+    <row r="98" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A98" s="13">
         <v>97</v>
       </c>
@@ -18757,20 +19150,24 @@
         <v>0</v>
       </c>
       <c r="R98" s="62">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="T98" s="37">
-        <v>0</v>
-      </c>
-      <c r="U98" s="16">
-        <v>1</v>
-      </c>
-      <c r="V98"/>
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="T98" s="106">
+        <f t="shared" si="3"/>
+        <v>3</v>
+      </c>
+      <c r="U98" s="37">
+        <v>0</v>
+      </c>
+      <c r="V98" s="16">
+        <v>1</v>
+      </c>
       <c r="W98"/>
       <c r="X98"/>
-    </row>
-    <row r="99" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="Y98"/>
+    </row>
+    <row r="99" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A99" s="13">
         <v>98</v>
       </c>
@@ -18823,20 +19220,24 @@
         <v>0</v>
       </c>
       <c r="R99" s="62">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="T99" s="37">
-        <v>0</v>
-      </c>
-      <c r="U99" s="16">
-        <v>0</v>
-      </c>
-      <c r="V99"/>
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="T99" s="106">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+      <c r="U99" s="37">
+        <v>0</v>
+      </c>
+      <c r="V99" s="16">
+        <v>0</v>
+      </c>
       <c r="W99"/>
       <c r="X99"/>
-    </row>
-    <row r="100" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="Y99"/>
+    </row>
+    <row r="100" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A100" s="13">
         <v>99</v>
       </c>
@@ -18889,20 +19290,24 @@
         <v>0</v>
       </c>
       <c r="R100" s="62">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="T100" s="37">
-        <v>0</v>
-      </c>
-      <c r="U100" s="16">
-        <v>1</v>
-      </c>
-      <c r="V100"/>
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="T100" s="106">
+        <f t="shared" si="3"/>
+        <v>3</v>
+      </c>
+      <c r="U100" s="37">
+        <v>0</v>
+      </c>
+      <c r="V100" s="16">
+        <v>1</v>
+      </c>
       <c r="W100"/>
       <c r="X100"/>
-    </row>
-    <row r="101" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="Y100"/>
+    </row>
+    <row r="101" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A101" s="23">
         <v>100</v>
       </c>
@@ -18955,20 +19360,24 @@
         <v>0</v>
       </c>
       <c r="R101" s="62">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="T101" s="37">
-        <v>0</v>
-      </c>
-      <c r="U101" s="16">
-        <v>0</v>
-      </c>
-      <c r="V101"/>
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="T101" s="106">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="U101" s="37">
+        <v>0</v>
+      </c>
+      <c r="V101" s="16">
+        <v>0</v>
+      </c>
       <c r="W101"/>
       <c r="X101"/>
-    </row>
-    <row r="102" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="Y101"/>
+    </row>
+    <row r="102" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A102" s="13">
         <v>101</v>
       </c>
@@ -19021,20 +19430,24 @@
         <v>0</v>
       </c>
       <c r="R102" s="62">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="T102" s="37">
-        <v>0</v>
-      </c>
-      <c r="U102" s="16">
-        <v>0</v>
-      </c>
-      <c r="V102"/>
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="T102" s="106">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+      <c r="U102" s="37">
+        <v>0</v>
+      </c>
+      <c r="V102" s="16">
+        <v>0</v>
+      </c>
       <c r="W102"/>
       <c r="X102"/>
-    </row>
-    <row r="103" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="Y102"/>
+    </row>
+    <row r="103" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A103" s="13">
         <v>102</v>
       </c>
@@ -19087,20 +19500,24 @@
         <v>0</v>
       </c>
       <c r="R103" s="62">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="T103" s="37">
-        <v>0</v>
-      </c>
-      <c r="U103" s="16">
-        <v>0</v>
-      </c>
-      <c r="V103"/>
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="T103" s="106">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+      <c r="U103" s="37">
+        <v>0</v>
+      </c>
+      <c r="V103" s="16">
+        <v>0</v>
+      </c>
       <c r="W103"/>
       <c r="X103"/>
-    </row>
-    <row r="104" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="Y103"/>
+    </row>
+    <row r="104" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A104" s="13">
         <v>103</v>
       </c>
@@ -19153,20 +19570,24 @@
         <v>0</v>
       </c>
       <c r="R104" s="62">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="T104" s="37">
-        <v>0</v>
-      </c>
-      <c r="U104" s="16">
-        <v>0</v>
-      </c>
-      <c r="V104"/>
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="T104" s="106">
+        <f t="shared" si="3"/>
+        <v>4</v>
+      </c>
+      <c r="U104" s="37">
+        <v>0</v>
+      </c>
+      <c r="V104" s="16">
+        <v>0</v>
+      </c>
       <c r="W104"/>
       <c r="X104"/>
-    </row>
-    <row r="105" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="Y104"/>
+    </row>
+    <row r="105" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A105" s="13">
         <v>104</v>
       </c>
@@ -19219,20 +19640,24 @@
         <v>0</v>
       </c>
       <c r="R105" s="62">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="T105" s="37">
-        <v>0</v>
-      </c>
-      <c r="U105" s="16">
-        <v>0</v>
-      </c>
-      <c r="V105"/>
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="T105" s="106">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+      <c r="U105" s="37">
+        <v>0</v>
+      </c>
+      <c r="V105" s="16">
+        <v>0</v>
+      </c>
       <c r="W105"/>
       <c r="X105"/>
-    </row>
-    <row r="106" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="Y105"/>
+    </row>
+    <row r="106" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A106" s="13">
         <v>105</v>
       </c>
@@ -19285,20 +19710,24 @@
         <v>0</v>
       </c>
       <c r="R106" s="62">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="T106" s="37">
-        <v>0</v>
-      </c>
-      <c r="U106" s="16">
-        <v>0</v>
-      </c>
-      <c r="V106"/>
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="T106" s="106">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="U106" s="37">
+        <v>0</v>
+      </c>
+      <c r="V106" s="16">
+        <v>0</v>
+      </c>
       <c r="W106"/>
       <c r="X106"/>
-    </row>
-    <row r="107" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="Y106"/>
+    </row>
+    <row r="107" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A107" s="13">
         <v>106</v>
       </c>
@@ -19351,20 +19780,24 @@
         <v>0</v>
       </c>
       <c r="R107" s="62">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="T107" s="37">
-        <v>0</v>
-      </c>
-      <c r="U107" s="16">
-        <v>0</v>
-      </c>
-      <c r="V107"/>
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="T107" s="106">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="U107" s="37">
+        <v>0</v>
+      </c>
+      <c r="V107" s="16">
+        <v>0</v>
+      </c>
       <c r="W107"/>
       <c r="X107"/>
-    </row>
-    <row r="108" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="Y107"/>
+    </row>
+    <row r="108" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A108" s="13">
         <v>107</v>
       </c>
@@ -19417,20 +19850,24 @@
         <v>0</v>
       </c>
       <c r="R108" s="62">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="T108" s="37">
-        <v>0</v>
-      </c>
-      <c r="U108" s="16">
-        <v>0</v>
-      </c>
-      <c r="V108"/>
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="T108" s="106">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="U108" s="37">
+        <v>0</v>
+      </c>
+      <c r="V108" s="16">
+        <v>0</v>
+      </c>
       <c r="W108"/>
       <c r="X108"/>
-    </row>
-    <row r="109" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="Y108"/>
+    </row>
+    <row r="109" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A109" s="13">
         <v>108</v>
       </c>
@@ -19483,20 +19920,24 @@
         <v>0</v>
       </c>
       <c r="R109" s="62">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="T109" s="37">
-        <v>0</v>
-      </c>
-      <c r="U109" s="16">
-        <v>0</v>
-      </c>
-      <c r="V109"/>
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="T109" s="106">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="U109" s="37">
+        <v>0</v>
+      </c>
+      <c r="V109" s="16">
+        <v>0</v>
+      </c>
       <c r="W109"/>
       <c r="X109"/>
-    </row>
-    <row r="110" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="Y109"/>
+    </row>
+    <row r="110" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A110" s="13">
         <v>109</v>
       </c>
@@ -19549,20 +19990,24 @@
         <v>0</v>
       </c>
       <c r="R110" s="62">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="T110" s="37">
-        <v>0</v>
-      </c>
-      <c r="U110" s="16">
-        <v>0</v>
-      </c>
-      <c r="V110"/>
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="T110" s="106">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="U110" s="37">
+        <v>0</v>
+      </c>
+      <c r="V110" s="16">
+        <v>0</v>
+      </c>
       <c r="W110"/>
       <c r="X110"/>
-    </row>
-    <row r="111" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="Y110"/>
+    </row>
+    <row r="111" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A111" s="13">
         <v>110</v>
       </c>
@@ -19615,20 +20060,24 @@
         <v>0</v>
       </c>
       <c r="R111" s="62">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="T111" s="37">
-        <v>0</v>
-      </c>
-      <c r="U111" s="16">
-        <v>0</v>
-      </c>
-      <c r="V111"/>
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="T111" s="106">
+        <f t="shared" si="3"/>
+        <v>5</v>
+      </c>
+      <c r="U111" s="37">
+        <v>0</v>
+      </c>
+      <c r="V111" s="16">
+        <v>0</v>
+      </c>
       <c r="W111"/>
       <c r="X111"/>
-    </row>
-    <row r="112" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="Y111"/>
+    </row>
+    <row r="112" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A112" s="13">
         <v>111</v>
       </c>
@@ -19681,20 +20130,24 @@
         <v>0</v>
       </c>
       <c r="R112" s="62">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="T112" s="37">
-        <v>0</v>
-      </c>
-      <c r="U112" s="16">
-        <v>0</v>
-      </c>
-      <c r="V112"/>
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="T112" s="106">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="U112" s="37">
+        <v>0</v>
+      </c>
+      <c r="V112" s="16">
+        <v>0</v>
+      </c>
       <c r="W112"/>
       <c r="X112"/>
-    </row>
-    <row r="113" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="Y112"/>
+    </row>
+    <row r="113" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A113" s="13">
         <v>112</v>
       </c>
@@ -19747,20 +20200,24 @@
         <v>0</v>
       </c>
       <c r="R113" s="62">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="T113" s="37">
-        <v>0</v>
-      </c>
-      <c r="U113" s="16">
-        <v>0</v>
-      </c>
-      <c r="V113"/>
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="T113" s="106">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="U113" s="37">
+        <v>0</v>
+      </c>
+      <c r="V113" s="16">
+        <v>0</v>
+      </c>
       <c r="W113"/>
       <c r="X113"/>
-    </row>
-    <row r="114" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="Y113"/>
+    </row>
+    <row r="114" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A114" s="13">
         <v>113</v>
       </c>
@@ -19813,20 +20270,24 @@
         <v>0</v>
       </c>
       <c r="R114" s="62">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="T114" s="37">
-        <v>0</v>
-      </c>
-      <c r="U114" s="16">
-        <v>0</v>
-      </c>
-      <c r="V114"/>
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="T114" s="106">
+        <f t="shared" si="3"/>
+        <v>3</v>
+      </c>
+      <c r="U114" s="37">
+        <v>0</v>
+      </c>
+      <c r="V114" s="16">
+        <v>0</v>
+      </c>
       <c r="W114"/>
       <c r="X114"/>
-    </row>
-    <row r="115" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="Y114"/>
+    </row>
+    <row r="115" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A115" s="23">
         <v>114</v>
       </c>
@@ -19879,20 +20340,24 @@
         <v>0</v>
       </c>
       <c r="R115" s="62">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="T115" s="37">
-        <v>0</v>
-      </c>
-      <c r="U115" s="16">
-        <v>0</v>
-      </c>
-      <c r="V115"/>
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="T115" s="106">
+        <f t="shared" si="3"/>
+        <v>3</v>
+      </c>
+      <c r="U115" s="37">
+        <v>0</v>
+      </c>
+      <c r="V115" s="16">
+        <v>0</v>
+      </c>
       <c r="W115"/>
       <c r="X115"/>
-    </row>
-    <row r="116" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="Y115"/>
+    </row>
+    <row r="116" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A116" s="13">
         <v>115</v>
       </c>
@@ -19945,20 +20410,24 @@
         <v>0</v>
       </c>
       <c r="R116" s="62">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="T116" s="37">
-        <v>0</v>
-      </c>
-      <c r="U116" s="16">
-        <v>0</v>
-      </c>
-      <c r="V116"/>
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="T116" s="106">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+      <c r="U116" s="37">
+        <v>0</v>
+      </c>
+      <c r="V116" s="16">
+        <v>0</v>
+      </c>
       <c r="W116"/>
       <c r="X116"/>
-    </row>
-    <row r="117" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="Y116"/>
+    </row>
+    <row r="117" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A117" s="27">
         <v>116</v>
       </c>
@@ -20011,20 +20480,24 @@
         <v>0</v>
       </c>
       <c r="R117" s="62">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="T117" s="37">
-        <v>0</v>
-      </c>
-      <c r="U117" s="16">
-        <v>0</v>
-      </c>
-      <c r="V117"/>
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="T117" s="106">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+      <c r="U117" s="37">
+        <v>0</v>
+      </c>
+      <c r="V117" s="16">
+        <v>0</v>
+      </c>
       <c r="W117"/>
       <c r="X117"/>
-    </row>
-    <row r="118" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="Y117"/>
+    </row>
+    <row r="118" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A118" s="27">
         <v>117</v>
       </c>
@@ -20077,20 +20550,24 @@
         <v>0</v>
       </c>
       <c r="R118" s="62">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="T118" s="37">
-        <v>0</v>
-      </c>
-      <c r="U118" s="16">
-        <v>0</v>
-      </c>
-      <c r="V118"/>
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="T118" s="106">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="U118" s="37">
+        <v>0</v>
+      </c>
+      <c r="V118" s="16">
+        <v>0</v>
+      </c>
       <c r="W118"/>
       <c r="X118"/>
-    </row>
-    <row r="119" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="Y118"/>
+    </row>
+    <row r="119" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A119" s="13">
         <v>118</v>
       </c>
@@ -20143,20 +20620,24 @@
         <v>0</v>
       </c>
       <c r="R119" s="62">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="T119" s="37">
-        <v>0</v>
-      </c>
-      <c r="U119" s="16">
-        <v>0</v>
-      </c>
-      <c r="V119"/>
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="T119" s="106">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="U119" s="37">
+        <v>0</v>
+      </c>
+      <c r="V119" s="16">
+        <v>0</v>
+      </c>
       <c r="W119"/>
       <c r="X119"/>
-    </row>
-    <row r="120" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="Y119"/>
+    </row>
+    <row r="120" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A120" s="13">
         <v>119</v>
       </c>
@@ -20209,20 +20690,24 @@
         <v>0</v>
       </c>
       <c r="R120" s="62">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="T120" s="37">
-        <v>0</v>
-      </c>
-      <c r="U120" s="16">
-        <v>0</v>
-      </c>
-      <c r="V120"/>
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="T120" s="106">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+      <c r="U120" s="37">
+        <v>0</v>
+      </c>
+      <c r="V120" s="16">
+        <v>0</v>
+      </c>
       <c r="W120"/>
       <c r="X120"/>
-    </row>
-    <row r="121" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="Y120"/>
+    </row>
+    <row r="121" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A121" s="13">
         <v>120</v>
       </c>
@@ -20275,20 +20760,24 @@
         <v>0</v>
       </c>
       <c r="R121" s="62">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="T121" s="37">
-        <v>0</v>
-      </c>
-      <c r="U121" s="16">
-        <v>0</v>
-      </c>
-      <c r="V121"/>
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="T121" s="106">
+        <f t="shared" si="3"/>
+        <v>3</v>
+      </c>
+      <c r="U121" s="37">
+        <v>0</v>
+      </c>
+      <c r="V121" s="16">
+        <v>0</v>
+      </c>
       <c r="W121"/>
       <c r="X121"/>
-    </row>
-    <row r="122" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="Y121"/>
+    </row>
+    <row r="122" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A122" s="13">
         <v>121</v>
       </c>
@@ -20341,20 +20830,24 @@
         <v>0</v>
       </c>
       <c r="R122" s="62">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="T122" s="37">
-        <v>0</v>
-      </c>
-      <c r="U122" s="16">
-        <v>0</v>
-      </c>
-      <c r="V122"/>
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="T122" s="106">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="U122" s="37">
+        <v>0</v>
+      </c>
+      <c r="V122" s="16">
+        <v>0</v>
+      </c>
       <c r="W122"/>
       <c r="X122"/>
-    </row>
-    <row r="123" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="Y122"/>
+    </row>
+    <row r="123" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A123" s="23">
         <v>122</v>
       </c>
@@ -20407,20 +20900,24 @@
         <v>0</v>
       </c>
       <c r="R123" s="62">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="T123" s="37">
-        <v>0</v>
-      </c>
-      <c r="U123" s="16">
-        <v>0</v>
-      </c>
-      <c r="V123"/>
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="T123" s="106">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="U123" s="37">
+        <v>0</v>
+      </c>
+      <c r="V123" s="16">
+        <v>0</v>
+      </c>
       <c r="W123"/>
       <c r="X123"/>
-    </row>
-    <row r="124" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="Y123"/>
+    </row>
+    <row r="124" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A124" s="13">
         <v>123</v>
       </c>
@@ -20473,20 +20970,24 @@
         <v>1</v>
       </c>
       <c r="R124" s="62">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="T124" s="37">
-        <v>0</v>
-      </c>
-      <c r="U124" s="16">
-        <v>0</v>
-      </c>
-      <c r="V124"/>
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="T124" s="106">
+        <f>SUM(H124:R124)</f>
+        <v>1</v>
+      </c>
+      <c r="U124" s="37">
+        <v>0</v>
+      </c>
+      <c r="V124" s="16">
+        <v>0</v>
+      </c>
       <c r="W124"/>
       <c r="X124"/>
-    </row>
-    <row r="125" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="Y124"/>
+    </row>
+    <row r="125" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A125" s="38">
         <v>124</v>
       </c>
@@ -20539,20 +21040,24 @@
         <v>0</v>
       </c>
       <c r="R125" s="62">
-        <f ca="1">SUM(Q125:T125)</f>
-        <v>0</v>
-      </c>
-      <c r="T125" s="49">
-        <v>0</v>
-      </c>
-      <c r="U125" s="42">
-        <v>0</v>
-      </c>
-      <c r="V125"/>
+        <f ca="1">SUM(Q125:U125)</f>
+        <v>0</v>
+      </c>
+      <c r="T125" s="106">
+        <f ca="1">SUM(H125:R125)</f>
+        <v>1</v>
+      </c>
+      <c r="U125" s="49">
+        <v>0</v>
+      </c>
+      <c r="V125" s="42">
+        <v>0</v>
+      </c>
       <c r="W125"/>
       <c r="X125"/>
-    </row>
-    <row r="127" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="Y125"/>
+    </row>
+    <row r="127" spans="1:25" x14ac:dyDescent="0.25">
       <c r="H127" s="50">
         <f>SUM(H2:H125)</f>
         <v>52</v>
@@ -20562,52 +21067,52 @@
         <v>47</v>
       </c>
       <c r="J127" s="50">
-        <f t="shared" ref="J127:T127" si="2">SUM(J2:J125)</f>
+        <f t="shared" ref="J127:U127" si="4">SUM(J2:J125)</f>
         <v>35</v>
       </c>
       <c r="K127" s="50">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>33</v>
       </c>
       <c r="L127" s="50">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>23</v>
       </c>
       <c r="M127" s="50">
-        <f t="shared" ref="M127:R127" si="3">SUM(M2:M125)</f>
+        <f t="shared" ref="M127:R127" si="5">SUM(M2:M125)</f>
         <v>12</v>
       </c>
       <c r="N127" s="50">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>11</v>
       </c>
       <c r="O127" s="50">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>8</v>
       </c>
       <c r="P127" s="50">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>7</v>
       </c>
       <c r="Q127" s="50">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>6</v>
       </c>
       <c r="R127" s="50">
-        <f t="shared" ca="1" si="3"/>
+        <f t="shared" ca="1" si="5"/>
         <v>8</v>
       </c>
-      <c r="T127" s="50">
-        <f t="shared" si="2"/>
+      <c r="U127" s="50">
+        <f t="shared" si="4"/>
         <v>4</v>
       </c>
-      <c r="U127" s="50">
-        <f>SUM(U2:U125)</f>
+      <c r="V127" s="50">
+        <f>SUM(V2:V125)</f>
         <v>4</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:X125" xr:uid="{4A5772B6-064D-45BE-A42A-53D0AD546609}"/>
+  <autoFilter ref="A1:Y125" xr:uid="{4A5772B6-064D-45BE-A42A-53D0AD546609}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>